<commit_message>
Remove Item support new map Fungle
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
   <si>
     <t>English</t>
   </si>
@@ -212,10 +212,10 @@
     <t>taskTextRoleIntroText</t>
   </si>
   <si>
-    <t>{0}Hover over ability buttons for more information.&lt;/color&gt;&lt;/color&gt;</t>
-  </si>
-  <si>
-    <t>{0}鼠标悬停在技能按键上获取更多信息.&lt;/color&gt;&lt;/color&gt;</t>
+    <t>{0}Hold down the right mouse button over ability buttons for more information.&lt;/color&gt;&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>{0}在技能按键上长按鼠标右键获取更多信息.&lt;/color&gt;&lt;/color&gt;</t>
   </si>
   <si>
     <t>HPSettings</t>
@@ -269,7 +269,7 @@
     <t>&lt;color=#FCDF04&gt;Random Game Start Position&lt;/color&gt;</t>
   </si>
   <si>
-    <t>&lt;color=#FCDF04&gt;开启随即出生点&lt;/color&gt;</t>
+    <t>&lt;color=#FCDF04&gt;开启随机出生点&lt;/color&gt;</t>
   </si>
   <si>
     <t>separateCooldowns</t>
@@ -541,13 +541,13 @@
     <t>The Killing Curse:
 A spell which will kill any target it hits, except Harry
 If the spell hits Harry, you will die instead
-&lt;#FF0000FF&gt;Right click to shoot this spell in the direction of your cursor</t>
+&lt;#FF0000FF&gt;Press the F key to shoot this spell in the direction of your cursor</t>
   </si>
   <si>
     <t>阿瓦达索命咒:
 一个可以杀死除哈利以外所有人的咒语。
 如果咒语击中哈利，你就会死亡。
-&lt;#FF0000FF&gt;右击可朝光标方向射出此咒语</t>
+&lt;#FF0000FF&gt;按下F按键可朝光标方向射出此咒语</t>
   </si>
   <si>
     <t>ButtonTextAvadacadavra</t>
@@ -727,6 +727,108 @@
     <t>模组作者: &lt;color=#00ffff&gt;FangkuaiYa&lt;/color&gt;
 &lt;#FFFFFFFF&gt;原作者: &lt;#7289DAFF&gt;Hunter101#1337
 &lt;#FFFFFFFF&gt;美工:&lt;color=#5A5AAD&gt;賣蟑螂&lt;/color&gt;&lt;color=#D3A4FF&gt;NotKomi&lt;/color&gt; &amp; &lt;#E67E22FF&gt;PhasmoFireGod&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>DeluminatorTooltip</t>
+  </si>
+  <si>
+    <t>Deluminator:
+Toggles the status of the lights (expect Fungle).</t>
+  </si>
+  <si>
+    <t>熄灯器:
+能够破坏灯光(除Fungle地图).</t>
+  </si>
+  <si>
+    <t>ElderWandTooltip</t>
+  </si>
+  <si>
+    <t>Elder Wand:
+If you are an Impostor, this
+item will reset your cooldowns to zero.
+Otherwise, you will get a single use button
+to kill anyone you think might be an Impostor</t>
+  </si>
+  <si>
+    <t>老魔杖:
+如果你是内鬼，你可以通过它重置你的冷却时间。
+反之则会获得一次杀死任何人的机会</t>
+  </si>
+  <si>
+    <t>GhostStoneTooltip</t>
+  </si>
+  <si>
+    <t>Resurrection Stone:
+Allows you to see ghosts.
+&lt;#FF0000FF&gt;This item cannot be consumed.</t>
+  </si>
+  <si>
+    <t>回魂石：
+可以让你看到灵魂玩家。
+&lt;#FF0000FF&gt;该物品为非消耗品.</t>
+  </si>
+  <si>
+    <t>MaraudersMapTooltip</t>
+  </si>
+  <si>
+    <t>Marauder's Map:
+Temporarily zooms out
+the camera. {0}s duration.</t>
+  </si>
+  <si>
+    <t>活点地图:
+扩大你的视野
+持续{0}秒.</t>
+  </si>
+  <si>
+    <t>PhiloStoneTooltip</t>
+  </si>
+  <si>
+    <t>Philosopher's Stone:
+This item will revive you when you die.
+&lt;#FF0000FF&gt;This item will be automatically consumed.</t>
+  </si>
+  <si>
+    <t>魔法石:
+当你死亡时,它会使你复活.
+&lt;#FF0000FF&gt;该物品会自动消耗的.</t>
+  </si>
+  <si>
+    <t>PortKeyTooltip</t>
+  </si>
+  <si>
+    <t>Port Key:
+Teleports you to\nthe emergency button.</t>
+  </si>
+  <si>
+    <t>门钥匙:
+使用后会将你传送到紧急会议的按钮旁边.</t>
+  </si>
+  <si>
+    <t>SortingHatTooltip</t>
+  </si>
+  <si>
+    <t>Sorting Hat:
+Reveals the role of the targeted player.
+&lt;#FF0000FF&gt;Can only be used in meetings!</t>
+  </si>
+  <si>
+    <t>分院帽:
+显示目标玩家的职业.
+&lt;#FF0000FF&gt;只能在会议中使用!</t>
+  </si>
+  <si>
+    <t>TheGoldenSnitchTooltip</t>
+  </si>
+  <si>
+    <t>The Golden Snitch:
+Forces all votes onto a targeted player.
+&lt;#FF0000FF&gt;Can only be used in meetings!</t>
+  </si>
+  <si>
+    <t>金色飞贼:
+将所有选票强制分配给目标玩家.
+&lt;#FF0000FF&gt;只能在会议中使用!</t>
   </si>
 </sst>
 </file>
@@ -1842,8 +1944,8 @@
   <sheetPr/>
   <dimension ref="A1:Z234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="O78" sqref="O78"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15"/>
@@ -4715,9 +4817,13 @@
       <c r="Y86" s="1"/>
       <c r="Z86" s="1"/>
     </row>
-    <row r="87" spans="1:26">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
+    <row r="87" ht="28.5" spans="1:26">
+      <c r="A87" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4730,7 +4836,9 @@
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
-      <c r="O87" s="1"/>
+      <c r="O87" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
@@ -4743,9 +4851,13 @@
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
     </row>
-    <row r="88" spans="1:26">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
+    <row r="88" ht="71.25" spans="1:26">
+      <c r="A88" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -4758,7 +4870,9 @@
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
-      <c r="O88" s="1"/>
+      <c r="O88" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
@@ -4771,9 +4885,13 @@
       <c r="Y88" s="1"/>
       <c r="Z88" s="1"/>
     </row>
-    <row r="89" spans="1:26">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
+    <row r="89" ht="42.75" spans="1:26">
+      <c r="A89" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>227</v>
+      </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -4786,7 +4904,9 @@
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
-      <c r="O89" s="1"/>
+      <c r="O89" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
@@ -4799,9 +4919,13 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" spans="1:26">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
+    <row r="90" ht="42.75" spans="1:26">
+      <c r="A90" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -4814,7 +4938,9 @@
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
-      <c r="O90" s="1"/>
+      <c r="O90" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
@@ -4827,9 +4953,13 @@
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" spans="1:26">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
+    <row r="91" ht="42.75" spans="1:26">
+      <c r="A91" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4842,7 +4972,9 @@
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
-      <c r="O91" s="1"/>
+      <c r="O91" s="2" t="s">
+        <v>234</v>
+      </c>
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
@@ -4855,9 +4987,13 @@
       <c r="Y91" s="1"/>
       <c r="Z91" s="1"/>
     </row>
-    <row r="92" spans="1:26">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
+    <row r="92" ht="28.5" spans="1:26">
+      <c r="A92" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -4870,7 +5006,9 @@
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
-      <c r="O92" s="1"/>
+      <c r="O92" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
@@ -4883,9 +5021,13 @@
       <c r="Y92" s="1"/>
       <c r="Z92" s="1"/>
     </row>
-    <row r="93" spans="1:26">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
+    <row r="93" ht="42.75" spans="1:26">
+      <c r="A93" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -4898,7 +5040,9 @@
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
-      <c r="O93" s="1"/>
+      <c r="O93" s="2" t="s">
+        <v>240</v>
+      </c>
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
@@ -4911,9 +5055,13 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
+    <row r="94" ht="42.75" spans="1:26">
+      <c r="A94" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>242</v>
+      </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -4926,7 +5074,9 @@
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
-      <c r="O94" s="1"/>
+      <c r="O94" s="2" t="s">
+        <v>243</v>
+      </c>
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>

</xml_diff>

<commit_message>
Version set to 2.2.0.
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="332">
   <si>
     <t>English</t>
   </si>
@@ -1216,6 +1216,24 @@
   <si>
     <t>蛇怪:
 撿到它的玩家會被石化直到下次會議結束</t>
+  </si>
+  <si>
+    <t>optionOn</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>开启</t>
+  </si>
+  <si>
+    <t>optionOff</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>关闭</t>
   </si>
 </sst>
 </file>
@@ -2354,8 +2372,8 @@
   <sheetPr/>
   <dimension ref="A1:Z231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C88" workbookViewId="0">
-      <selection activeCell="O91" sqref="O91"/>
+    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
+      <selection activeCell="O102" sqref="O102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15"/>
@@ -5844,8 +5862,12 @@
       <c r="Z100" s="1"/>
     </row>
     <row r="101" spans="1:26">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
+      <c r="A101" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -5858,7 +5880,9 @@
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
+      <c r="O101" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
@@ -5872,8 +5896,12 @@
       <c r="Z101" s="1"/>
     </row>
     <row r="102" spans="1:26">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
+      <c r="A102" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -5886,7 +5914,9 @@
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
+      <c r="O102" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>

</xml_diff>